<commit_message>
Sprint 6 y diagrama de actividades
</commit_message>
<xml_diff>
--- a/Documentación/3. Historia de Usuario/Historias de usuario_ver_3.xlsx
+++ b/Documentación/3. Historia de Usuario/Historias de usuario_ver_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Scarlet\Documentación\3. Historia de Usuario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DEE3E4-579C-40B4-A2CB-8246351A1677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98C4736-5C25-4FA9-BF0C-AC84A394B43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1369,49 +1369,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1423,6 +1398,39 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1430,6 +1438,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1454,27 +1465,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1697,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="A17:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1727,12 +1727,12 @@
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
-      <c r="G1" s="76" t="s">
+      <c r="G1" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
       <c r="K1" s="17"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1808,29 +1808,29 @@
     </row>
     <row r="4" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="69" t="s">
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="65" t="s">
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="69" t="s">
+      <c r="L4" s="74" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="69" t="s">
+      <c r="M4" s="74" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="69" t="s">
+      <c r="N4" s="74" t="s">
         <v>43</v>
       </c>
       <c r="O4" s="1"/>
@@ -1875,10 +1875,10 @@
       <c r="J5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="66"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
@@ -1894,22 +1894,22 @@
     </row>
     <row r="6" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="52" t="s">
+      <c r="D6" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="54" t="s">
         <v>50</v>
       </c>
       <c r="F6" s="24">
         <v>1</v>
       </c>
-      <c r="G6" s="77" t="s">
+      <c r="G6" s="47" t="s">
         <v>169</v>
       </c>
       <c r="H6" s="36" t="s">
@@ -1918,7 +1918,7 @@
       <c r="I6" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="J6" s="77" t="s">
+      <c r="J6" s="47" t="s">
         <v>172</v>
       </c>
       <c r="K6" s="38" t="s">
@@ -1927,10 +1927,10 @@
       <c r="L6" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="47">
+      <c r="M6" s="66">
         <v>6</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="54" t="s">
         <v>55</v>
       </c>
       <c r="O6" s="1"/>
@@ -1948,23 +1948,23 @@
     </row>
     <row r="7" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="24">
         <v>2</v>
       </c>
-      <c r="G7" s="77" t="s">
+      <c r="G7" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="H7" s="77" t="s">
+      <c r="H7" s="47" t="s">
         <v>51</v>
       </c>
       <c r="I7" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="J7" s="77" t="s">
+      <c r="J7" s="47" t="s">
         <v>168</v>
       </c>
       <c r="K7" s="38" t="s">
@@ -1973,8 +1973,8 @@
       <c r="L7" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="48"/>
-      <c r="N7" s="52"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="54"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
@@ -1990,19 +1990,19 @@
     </row>
     <row r="8" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="73"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
+      <c r="N8" s="78"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -2018,31 +2018,31 @@
     </row>
     <row r="9" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="52" t="s">
+      <c r="B9" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="54" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="52" t="s">
+      <c r="D9" s="54" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="78">
+      <c r="F9" s="48">
         <v>1</v>
       </c>
-      <c r="G9" s="78" t="s">
+      <c r="G9" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="77" t="s">
+      <c r="I9" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="J9" s="77" t="s">
+      <c r="J9" s="47" t="s">
         <v>183</v>
       </c>
       <c r="K9" s="43" t="s">
@@ -2051,10 +2051,10 @@
       <c r="L9" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="M9" s="47">
+      <c r="M9" s="66">
         <v>6</v>
       </c>
-      <c r="N9" s="47" t="s">
+      <c r="N9" s="66" t="s">
         <v>62</v>
       </c>
       <c r="O9" s="1"/>
@@ -2072,23 +2072,23 @@
     </row>
     <row r="10" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="78">
+      <c r="B10" s="54"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="48">
         <v>2</v>
       </c>
-      <c r="G10" s="78" t="s">
+      <c r="G10" s="48" t="s">
         <v>176</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="77" t="s">
+      <c r="I10" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="J10" s="77" t="s">
+      <c r="J10" s="47" t="s">
         <v>184</v>
       </c>
       <c r="K10" s="43" t="s">
@@ -2097,8 +2097,8 @@
       <c r="L10" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -2114,19 +2114,19 @@
     </row>
     <row r="11" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="70"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="60"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="65"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -2160,7 +2160,7 @@
       <c r="G12" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="H12" s="79" t="s">
+      <c r="H12" s="49" t="s">
         <v>177</v>
       </c>
       <c r="I12" s="40" t="s">
@@ -2196,19 +2196,19 @@
     </row>
     <row r="13" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="67"/>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-      <c r="M13" s="67"/>
-      <c r="N13" s="67"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="71"/>
+      <c r="N13" s="71"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
@@ -2278,19 +2278,19 @@
     </row>
     <row r="15" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="57"/>
+      <c r="B15" s="72"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="61"/>
+      <c r="N15" s="62"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
@@ -2306,43 +2306,43 @@
     </row>
     <row r="16" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="50" t="s">
         <v>81</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="80" t="s">
+      <c r="D16" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="80" t="s">
+      <c r="E16" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="F16" s="80">
+      <c r="F16" s="50">
         <v>1</v>
       </c>
-      <c r="G16" s="80" t="s">
+      <c r="G16" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="H16" s="80" t="s">
+      <c r="H16" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="I16" s="80" t="s">
+      <c r="I16" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="J16" s="80" t="s">
+      <c r="J16" s="50" t="s">
         <v>185</v>
       </c>
-      <c r="K16" s="80" t="s">
+      <c r="K16" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="L16" s="80" t="s">
+      <c r="L16" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="80">
+      <c r="M16" s="50">
         <v>4</v>
       </c>
-      <c r="N16" s="80" t="s">
+      <c r="N16" s="50" t="s">
         <v>186</v>
       </c>
       <c r="O16" s="1"/>
@@ -2360,19 +2360,19 @@
     </row>
     <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="56"/>
-      <c r="H17" s="56"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="57"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="62"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -2386,75 +2386,75 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" s="83" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="82"/>
-      <c r="B18" s="80" t="s">
+    <row r="18" spans="1:26" s="52" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="50" t="s">
         <v>95</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="80" t="s">
+      <c r="D18" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="E18" s="80" t="s">
+      <c r="E18" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="F18" s="80">
+      <c r="F18" s="50">
         <v>1</v>
       </c>
-      <c r="G18" s="80" t="s">
+      <c r="G18" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="H18" s="80" t="s">
+      <c r="H18" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="I18" s="80" t="s">
+      <c r="I18" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="J18" s="80" t="s">
+      <c r="J18" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="K18" s="80" t="s">
+      <c r="K18" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="L18" s="80" t="s">
+      <c r="L18" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="M18" s="80">
+      <c r="M18" s="50">
         <v>2</v>
       </c>
-      <c r="N18" s="80" t="s">
+      <c r="N18" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="O18" s="82"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="82"/>
-      <c r="T18" s="82"/>
-      <c r="U18" s="82"/>
-      <c r="V18" s="82"/>
-      <c r="W18" s="82"/>
-      <c r="X18" s="82"/>
-      <c r="Y18" s="82"/>
-      <c r="Z18" s="82"/>
+      <c r="O18" s="51"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="51"/>
+      <c r="R18" s="51"/>
+      <c r="S18" s="51"/>
+      <c r="T18" s="51"/>
+      <c r="U18" s="51"/>
+      <c r="V18" s="51"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="51"/>
+      <c r="Z18" s="51"/>
     </row>
     <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-      <c r="N19" s="81"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -2468,75 +2468,75 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" s="83" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="82"/>
-      <c r="B20" s="84" t="s">
+    <row r="20" spans="1:26" s="52" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="51"/>
+      <c r="B20" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="84" t="s">
+      <c r="C20" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="84" t="s">
+      <c r="D20" s="53" t="s">
         <v>193</v>
       </c>
-      <c r="E20" s="84" t="s">
+      <c r="E20" s="53" t="s">
         <v>194</v>
       </c>
-      <c r="F20" s="80">
+      <c r="F20" s="50">
         <v>1</v>
       </c>
-      <c r="G20" s="80" t="s">
+      <c r="G20" s="50" t="s">
         <v>195</v>
       </c>
-      <c r="H20" s="80" t="s">
+      <c r="H20" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="I20" s="80" t="s">
+      <c r="I20" s="50" t="s">
         <v>197</v>
       </c>
-      <c r="J20" s="80" t="s">
+      <c r="J20" s="50" t="s">
         <v>198</v>
       </c>
-      <c r="K20" s="80" t="s">
+      <c r="K20" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="L20" s="80" t="s">
+      <c r="L20" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="80">
+      <c r="M20" s="50">
         <v>4</v>
       </c>
-      <c r="N20" s="80" t="s">
+      <c r="N20" s="50" t="s">
         <v>192</v>
       </c>
-      <c r="O20" s="82"/>
-      <c r="P20" s="82"/>
-      <c r="Q20" s="82"/>
-      <c r="R20" s="82"/>
-      <c r="S20" s="82"/>
-      <c r="T20" s="82"/>
-      <c r="U20" s="82"/>
-      <c r="V20" s="82"/>
-      <c r="W20" s="82"/>
-      <c r="X20" s="82"/>
-      <c r="Y20" s="82"/>
-      <c r="Z20" s="82"/>
+      <c r="O20" s="51"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="51"/>
+      <c r="S20" s="51"/>
+      <c r="T20" s="51"/>
+      <c r="U20" s="51"/>
+      <c r="V20" s="51"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
     </row>
     <row r="21" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="57"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="61"/>
+      <c r="N21" s="62"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -2552,16 +2552,16 @@
     </row>
     <row r="22" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="58" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="58" t="s">
         <v>84</v>
       </c>
       <c r="F22" s="16">
@@ -2585,10 +2585,10 @@
       <c r="L22" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="M22" s="68">
+      <c r="M22" s="73">
         <v>6</v>
       </c>
-      <c r="N22" s="68" t="s">
+      <c r="N22" s="73" t="s">
         <v>80</v>
       </c>
       <c r="O22" s="1"/>
@@ -2606,10 +2606,10 @@
     </row>
     <row r="23" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
       <c r="F23" s="16">
         <v>2</v>
       </c>
@@ -2631,8 +2631,8 @@
       <c r="L23" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="M23" s="68"/>
-      <c r="N23" s="68"/>
+      <c r="M23" s="73"/>
+      <c r="N23" s="73"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -2648,10 +2648,10 @@
     </row>
     <row r="24" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
       <c r="F24" s="16">
         <v>3</v>
       </c>
@@ -2673,8 +2673,8 @@
       <c r="L24" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -2690,19 +2690,19 @@
     </row>
     <row r="25" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="57"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="62"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -2772,19 +2772,19 @@
     </row>
     <row r="27" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="60"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="65"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2800,43 +2800,43 @@
     </row>
     <row r="28" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="B28" s="80" t="s">
+      <c r="B28" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="C28" s="80" t="s">
+      <c r="C28" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="80" t="s">
+      <c r="D28" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="E28" s="80" t="s">
+      <c r="E28" s="50" t="s">
         <v>201</v>
       </c>
-      <c r="F28" s="80">
+      <c r="F28" s="50">
         <v>1</v>
       </c>
-      <c r="G28" s="77" t="s">
+      <c r="G28" s="47" t="s">
         <v>202</v>
       </c>
-      <c r="H28" s="80" t="s">
+      <c r="H28" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="I28" s="80" t="s">
+      <c r="I28" s="50" t="s">
         <v>204</v>
       </c>
-      <c r="J28" s="80" t="s">
+      <c r="J28" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="K28" s="80" t="s">
+      <c r="K28" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="L28" s="80" t="s">
+      <c r="L28" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="M28" s="80">
+      <c r="M28" s="50">
         <v>6</v>
       </c>
-      <c r="N28" s="80" t="s">
+      <c r="N28" s="50" t="s">
         <v>214</v>
       </c>
       <c r="O28" s="1"/>
@@ -2854,19 +2854,19 @@
     </row>
     <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="60"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="65"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -2882,16 +2882,16 @@
     </row>
     <row r="30" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="49" t="s">
+      <c r="B30" s="58" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="49" t="s">
+      <c r="E30" s="58" t="s">
         <v>105</v>
       </c>
       <c r="F30" s="16">
@@ -2915,10 +2915,10 @@
       <c r="L30" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="M30" s="47">
+      <c r="M30" s="66">
         <v>6</v>
       </c>
-      <c r="N30" s="47" t="s">
+      <c r="N30" s="66" t="s">
         <v>110</v>
       </c>
       <c r="O30" s="1"/>
@@ -2936,10 +2936,10 @@
     </row>
     <row r="31" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
       <c r="F31" s="16">
         <v>2</v>
       </c>
@@ -2961,8 +2961,8 @@
       <c r="L31" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="M31" s="48"/>
-      <c r="N31" s="48"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
@@ -2978,19 +2978,19 @@
     </row>
     <row r="32" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="56"/>
-      <c r="H32" s="56"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="56"/>
-      <c r="K32" s="56"/>
-      <c r="L32" s="56"/>
-      <c r="M32" s="56"/>
-      <c r="N32" s="57"/>
+      <c r="B32" s="72"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="62"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -3006,43 +3006,43 @@
     </row>
     <row r="33" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="80" t="s">
+      <c r="B33" s="50" t="s">
         <v>199</v>
       </c>
-      <c r="C33" s="80" t="s">
+      <c r="C33" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="80" t="s">
+      <c r="D33" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="E33" s="80" t="s">
+      <c r="E33" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="F33" s="80">
+      <c r="F33" s="50">
         <v>1</v>
       </c>
-      <c r="G33" s="80" t="s">
+      <c r="G33" s="50" t="s">
         <v>209</v>
       </c>
-      <c r="H33" s="80" t="s">
+      <c r="H33" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="I33" s="80" t="s">
+      <c r="I33" s="50" t="s">
         <v>210</v>
       </c>
-      <c r="J33" s="80" t="s">
+      <c r="J33" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="K33" s="80" t="s">
+      <c r="K33" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="L33" s="80" t="s">
+      <c r="L33" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="M33" s="80">
+      <c r="M33" s="50">
         <v>6</v>
       </c>
-      <c r="N33" s="80" t="s">
+      <c r="N33" s="50" t="s">
         <v>213</v>
       </c>
       <c r="O33" s="1"/>
@@ -3060,19 +3060,19 @@
     </row>
     <row r="34" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="63"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="63"/>
+      <c r="N34" s="63"/>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
@@ -3088,16 +3088,16 @@
     </row>
     <row r="35" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="52" t="s">
+      <c r="B35" s="54" t="s">
         <v>200</v>
       </c>
-      <c r="C35" s="52" t="s">
+      <c r="C35" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="52" t="s">
+      <c r="D35" s="54" t="s">
         <v>116</v>
       </c>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="54" t="s">
         <v>117</v>
       </c>
       <c r="F35" s="16">
@@ -3121,10 +3121,10 @@
       <c r="L35" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="M35" s="47">
+      <c r="M35" s="66">
         <v>24</v>
       </c>
-      <c r="N35" s="49" t="s">
+      <c r="N35" s="58" t="s">
         <v>122</v>
       </c>
       <c r="O35" s="1"/>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="36" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="52"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="54"/>
       <c r="F36" s="16">
         <v>2</v>
       </c>
@@ -3167,8 +3167,8 @@
       <c r="L36" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="M36" s="48"/>
-      <c r="N36" s="51"/>
+      <c r="M36" s="67"/>
+      <c r="N36" s="59"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -3184,19 +3184,19 @@
     </row>
     <row r="37" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="56"/>
-      <c r="M37" s="56"/>
-      <c r="N37" s="57"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="62"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
@@ -3212,16 +3212,16 @@
     </row>
     <row r="38" spans="1:26" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="49" t="s">
+      <c r="B38" s="58" t="s">
         <v>215</v>
       </c>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="58" t="s">
         <v>129</v>
       </c>
       <c r="F38" s="35">
@@ -3245,10 +3245,10 @@
       <c r="L38" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="M38" s="49">
+      <c r="M38" s="58">
         <v>4</v>
       </c>
-      <c r="N38" s="49" t="s">
+      <c r="N38" s="58" t="s">
         <v>138</v>
       </c>
       <c r="O38" s="1"/>
@@ -3266,10 +3266,10 @@
     </row>
     <row r="39" spans="1:26" ht="92.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="51"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="E39" s="59"/>
       <c r="F39" s="35">
         <v>2</v>
       </c>
@@ -3291,8 +3291,8 @@
       <c r="L39" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
+      <c r="M39" s="59"/>
+      <c r="N39" s="59"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
@@ -3308,19 +3308,19 @@
     </row>
     <row r="40" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="B40" s="61"/>
-      <c r="C40" s="56"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="56"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="56"/>
-      <c r="M40" s="56"/>
-      <c r="N40" s="57"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="61"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="62"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
@@ -3336,16 +3336,16 @@
     </row>
     <row r="41" spans="1:26" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="49" t="s">
+      <c r="B41" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="58" t="s">
         <v>140</v>
       </c>
-      <c r="E41" s="49" t="s">
+      <c r="E41" s="58" t="s">
         <v>141</v>
       </c>
       <c r="F41" s="16">
@@ -3369,10 +3369,10 @@
       <c r="L41" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="M41" s="49">
+      <c r="M41" s="58">
         <v>12</v>
       </c>
-      <c r="N41" s="49" t="s">
+      <c r="N41" s="58" t="s">
         <v>154</v>
       </c>
       <c r="O41" s="1"/>
@@ -3390,10 +3390,10 @@
     </row>
     <row r="42" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="50"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="81"/>
+      <c r="E42" s="81"/>
       <c r="F42" s="16">
         <v>2</v>
       </c>
@@ -3415,8 +3415,8 @@
       <c r="L42" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="M42" s="50"/>
-      <c r="N42" s="50"/>
+      <c r="M42" s="81"/>
+      <c r="N42" s="81"/>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -3432,10 +3432,10 @@
     </row>
     <row r="43" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="51"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
       <c r="F43" s="16">
         <v>3</v>
       </c>
@@ -3457,8 +3457,8 @@
       <c r="L43" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="M43" s="51"/>
-      <c r="N43" s="51"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
@@ -3474,19 +3474,19 @@
     </row>
     <row r="44" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
-      <c r="B44" s="62"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="63"/>
-      <c r="K44" s="63"/>
-      <c r="L44" s="63"/>
-      <c r="M44" s="63"/>
-      <c r="N44" s="64"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="56"/>
+      <c r="K44" s="56"/>
+      <c r="L44" s="56"/>
+      <c r="M44" s="56"/>
+      <c r="N44" s="57"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
@@ -3502,16 +3502,16 @@
     </row>
     <row r="45" spans="1:26" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
-      <c r="B45" s="49" t="s">
+      <c r="B45" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C45" s="52" t="s">
+      <c r="C45" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="D45" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="E45" s="49" t="s">
+      <c r="E45" s="58" t="s">
         <v>157</v>
       </c>
       <c r="F45" s="16">
@@ -3535,10 +3535,10 @@
       <c r="L45" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="M45" s="47">
+      <c r="M45" s="66">
         <v>8</v>
       </c>
-      <c r="N45" s="47" t="s">
+      <c r="N45" s="66" t="s">
         <v>167</v>
       </c>
       <c r="O45" s="1"/>
@@ -3556,10 +3556,10 @@
     </row>
     <row r="46" spans="1:26" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
-      <c r="B46" s="51"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="51"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="84"/>
+      <c r="E46" s="59"/>
       <c r="F46" s="16">
         <v>2</v>
       </c>
@@ -3581,8 +3581,8 @@
       <c r="L46" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
+      <c r="M46" s="67"/>
+      <c r="N46" s="67"/>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
@@ -3598,19 +3598,19 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
-      <c r="B47" s="62"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="63"/>
-      <c r="L47" s="63"/>
-      <c r="M47" s="63"/>
-      <c r="N47" s="64"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="56"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="57"/>
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
@@ -3626,16 +3626,16 @@
     </row>
     <row r="48" spans="1:26" s="18" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A48" s="17"/>
-      <c r="B48" s="52" t="s">
+      <c r="B48" s="54" t="s">
         <v>229</v>
       </c>
-      <c r="C48" s="52" t="s">
+      <c r="C48" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="D48" s="52" t="s">
+      <c r="D48" s="54" t="s">
         <v>216</v>
       </c>
-      <c r="E48" s="52" t="s">
+      <c r="E48" s="54" t="s">
         <v>217</v>
       </c>
       <c r="F48" s="43">
@@ -3659,10 +3659,10 @@
       <c r="L48" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="M48" s="49">
+      <c r="M48" s="58">
         <v>8</v>
       </c>
-      <c r="N48" s="49" t="s">
+      <c r="N48" s="58" t="s">
         <v>222</v>
       </c>
       <c r="O48" s="17"/>
@@ -3680,10 +3680,10 @@
     </row>
     <row r="49" spans="1:26" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="17"/>
-      <c r="B49" s="52"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="52"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
       <c r="F49" s="43">
         <v>2</v>
       </c>
@@ -3705,8 +3705,8 @@
       <c r="L49" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="M49" s="51"/>
-      <c r="N49" s="51"/>
+      <c r="M49" s="59"/>
+      <c r="N49" s="59"/>
       <c r="O49" s="17"/>
       <c r="P49" s="17"/>
       <c r="Q49" s="17"/>
@@ -3722,19 +3722,19 @@
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="63"/>
-      <c r="E50" s="63"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="63"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="63"/>
-      <c r="J50" s="63"/>
-      <c r="K50" s="63"/>
-      <c r="L50" s="63"/>
-      <c r="M50" s="63"/>
-      <c r="N50" s="64"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
+      <c r="N50" s="57"/>
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="1"/>
@@ -3750,16 +3750,16 @@
     </row>
     <row r="51" spans="1:26" s="18" customFormat="1" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17"/>
-      <c r="B51" s="52" t="s">
+      <c r="B51" s="54" t="s">
         <v>231</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="54" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="52" t="s">
+      <c r="D51" s="54" t="s">
         <v>230</v>
       </c>
-      <c r="E51" s="52" t="s">
+      <c r="E51" s="54" t="s">
         <v>232</v>
       </c>
       <c r="F51" s="43">
@@ -3777,16 +3777,16 @@
       <c r="J51" s="43" t="s">
         <v>240</v>
       </c>
-      <c r="K51" s="52" t="s">
+      <c r="K51" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="L51" s="52" t="s">
+      <c r="L51" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="M51" s="52">
+      <c r="M51" s="54">
         <v>8</v>
       </c>
-      <c r="N51" s="52" t="s">
+      <c r="N51" s="54" t="s">
         <v>236</v>
       </c>
       <c r="O51" s="17"/>
@@ -3804,10 +3804,10 @@
     </row>
     <row r="52" spans="1:26" s="18" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="17"/>
-      <c r="B52" s="52"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
       <c r="F52" s="43">
         <v>2</v>
       </c>
@@ -3823,10 +3823,10 @@
       <c r="J52" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="K52" s="52"/>
-      <c r="L52" s="52"/>
-      <c r="M52" s="52"/>
-      <c r="N52" s="52"/>
+      <c r="K52" s="54"/>
+      <c r="L52" s="54"/>
+      <c r="M52" s="54"/>
+      <c r="N52" s="54"/>
       <c r="O52" s="17"/>
       <c r="P52" s="17"/>
       <c r="Q52" s="17"/>
@@ -3842,19 +3842,19 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
-      <c r="B53" s="62"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
-      <c r="E53" s="63"/>
-      <c r="F53" s="63"/>
-      <c r="G53" s="63"/>
-      <c r="H53" s="63"/>
-      <c r="I53" s="63"/>
-      <c r="J53" s="63"/>
-      <c r="K53" s="63"/>
-      <c r="L53" s="63"/>
-      <c r="M53" s="63"/>
-      <c r="N53" s="64"/>
+      <c r="B53" s="55"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="56"/>
+      <c r="N53" s="57"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="1"/>
@@ -29499,41 +29499,39 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="L51:L52"/>
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="N51:N52"/>
-    <mergeCell ref="B50:N50"/>
-    <mergeCell ref="B53:N53"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="K51:K52"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="B47:N47"/>
-    <mergeCell ref="M48:M49"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="B17:N17"/>
-    <mergeCell ref="B19:N19"/>
-    <mergeCell ref="B21:N21"/>
-    <mergeCell ref="B29:N29"/>
-    <mergeCell ref="B34:N34"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="N45:N46"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="M41:M43"/>
+    <mergeCell ref="N41:N43"/>
+    <mergeCell ref="E41:E43"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="B44:N44"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="M35:M36"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="B37:N37"/>
+    <mergeCell ref="B40:N40"/>
+    <mergeCell ref="M30:M31"/>
+    <mergeCell ref="N30:N31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="N35:N36"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="M38:M39"/>
+    <mergeCell ref="N38:N39"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="B13:N13"/>
     <mergeCell ref="B15:N15"/>
@@ -29550,42 +29548,44 @@
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="E22:E24"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="B17:N17"/>
+    <mergeCell ref="B19:N19"/>
+    <mergeCell ref="B21:N21"/>
+    <mergeCell ref="B29:N29"/>
+    <mergeCell ref="B34:N34"/>
     <mergeCell ref="B25:N25"/>
     <mergeCell ref="B27:N27"/>
     <mergeCell ref="B32:N32"/>
-    <mergeCell ref="B37:N37"/>
-    <mergeCell ref="B40:N40"/>
-    <mergeCell ref="M30:M31"/>
-    <mergeCell ref="N30:N31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="N35:N36"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="N38:N39"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="M35:M36"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="N45:N46"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="M41:M43"/>
-    <mergeCell ref="N41:N43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="B44:N44"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="B47:N47"/>
+    <mergeCell ref="M48:M49"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="L51:L52"/>
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="N51:N52"/>
+    <mergeCell ref="B50:N50"/>
+    <mergeCell ref="B53:N53"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="K51:K52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>